<commit_message>
final object import attempt 1
</commit_message>
<xml_diff>
--- a/data/properties_other.xlsx
+++ b/data/properties_other.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katie/MetadataLab/LinkedArchives/Linked_Archives_Wikibase/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{74557FD0-5870-5345-B9FF-9F15EE2A36AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A9C878-7E86-E643-B135-E20ECF3CE1F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="460" windowWidth="24820" windowHeight="16280"/>
+    <workbookView xWindow="260" yWindow="460" windowWidth="22060" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="properties" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="334">
   <si>
     <t>described by source</t>
   </si>
@@ -156,9 +156,6 @@
     <t>P163</t>
   </si>
   <si>
-    <t>P172</t>
-  </si>
-  <si>
     <t>P166</t>
   </si>
   <si>
@@ -240,57 +237,15 @@
     <t>P1705</t>
   </si>
   <si>
-    <t>capital of</t>
-  </si>
-  <si>
-    <t>P1376</t>
-  </si>
-  <si>
-    <t>director</t>
-  </si>
-  <si>
-    <t>P57</t>
-  </si>
-  <si>
-    <t>screenwriter</t>
-  </si>
-  <si>
-    <t>P58</t>
-  </si>
-  <si>
     <t>P136</t>
   </si>
   <si>
-    <t>original language of film or TV show</t>
-  </si>
-  <si>
-    <t>P364</t>
-  </si>
-  <si>
     <t>country of origin</t>
   </si>
   <si>
     <t>P495</t>
   </si>
   <si>
-    <t>publication date</t>
-  </si>
-  <si>
-    <t>P577</t>
-  </si>
-  <si>
-    <t>distributed by</t>
-  </si>
-  <si>
-    <t>P750</t>
-  </si>
-  <si>
-    <t>copyright status</t>
-  </si>
-  <si>
-    <t>P6216</t>
-  </si>
-  <si>
     <t>subclass of</t>
   </si>
   <si>
@@ -303,96 +258,27 @@
     <t>P156</t>
   </si>
   <si>
-    <t>P175</t>
-  </si>
-  <si>
     <t>P140</t>
   </si>
   <si>
-    <t>composer</t>
-  </si>
-  <si>
-    <t>P86</t>
-  </si>
-  <si>
-    <t>librettist</t>
-  </si>
-  <si>
-    <t>P87</t>
-  </si>
-  <si>
-    <t>P171</t>
-  </si>
-  <si>
-    <t>lyrics by</t>
-  </si>
-  <si>
-    <t>P676</t>
-  </si>
-  <si>
     <t>P144</t>
   </si>
   <si>
-    <t>tonality</t>
-  </si>
-  <si>
-    <t>P826</t>
-  </si>
-  <si>
-    <t>event interval</t>
-  </si>
-  <si>
-    <t>P2257</t>
-  </si>
-  <si>
-    <t>location</t>
-  </si>
-  <si>
-    <t>P276</t>
-  </si>
-  <si>
     <t>P137</t>
   </si>
   <si>
-    <t>P176</t>
-  </si>
-  <si>
-    <t>length</t>
-  </si>
-  <si>
-    <t>P2043</t>
-  </si>
-  <si>
-    <t>organizer</t>
-  </si>
-  <si>
-    <t>P664</t>
-  </si>
-  <si>
-    <t>P179</t>
-  </si>
-  <si>
     <t>located on terrain feature</t>
   </si>
   <si>
     <t>P706</t>
   </si>
   <si>
-    <t>duration</t>
-  </si>
-  <si>
-    <t>P2047</t>
-  </si>
-  <si>
     <t>P161</t>
   </si>
   <si>
     <t>P162</t>
   </si>
   <si>
-    <t>P170</t>
-  </si>
-  <si>
     <t>health specialty</t>
   </si>
   <si>
@@ -441,21 +327,12 @@
     <t>next higher class or type; all instances of these items are instances of those items; this item is a class (subset) of that item</t>
   </si>
   <si>
-    <t>date or point in time when a work was first published or released</t>
-  </si>
-  <si>
     <t>date or point in time when the subject came into existence as defined</t>
   </si>
   <si>
-    <t>person(s) who wrote the music</t>
-  </si>
-  <si>
     <t>type of agents that study this subject or work in this profession</t>
   </si>
   <si>
-    <t>copyright status for intellectual creations like works of art, publications, software, etc.</t>
-  </si>
-  <si>
     <t>sovereign state of this item</t>
   </si>
   <si>
@@ -474,9 +351,6 @@
     <t>continent of which the subject is a part</t>
   </si>
   <si>
-    <t>primary city of a country, province, state or other type of administrative territorial entity</t>
-  </si>
-  <si>
     <t>language designated as official by this item</t>
   </si>
   <si>
@@ -495,9 +369,6 @@
     <t>short name of a place, organisation, person, Wikidata property, etc.</t>
   </si>
   <si>
-    <t>country's total GDP divided by the population</t>
-  </si>
-  <si>
     <t>number of people inhabiting the place; number of people of subject</t>
   </si>
   <si>
@@ -516,36 +387,21 @@
     <t>main specialty that diagnoses, prevent human illness, injury and other physical and mental impairments</t>
   </si>
   <si>
-    <t>official with the highest formal authority in a country/state</t>
-  </si>
-  <si>
     <t>official name of the subject in its official language(s)</t>
   </si>
   <si>
-    <t>countries or administrative subdivisions, of equal level, that this item borders, either by land or water</t>
-  </si>
-  <si>
     <t>political office that is fulfilled by the head of state of this item</t>
   </si>
   <si>
     <t>supreme judicial body within a country, administrative division, or other organization</t>
   </si>
   <si>
-    <t>country, state, department, canton or other administrative division of which the municipality is the governmental seat</t>
-  </si>
-  <si>
     <t>person(s) who wrote the script for subject item</t>
   </si>
   <si>
     <t>language in which a film or a performance work was originally created</t>
   </si>
   <si>
-    <t>country of origin of this item</t>
-  </si>
-  <si>
-    <t>distributor of a creative work; distributor for a record label; news agency; film distributor</t>
-  </si>
-  <si>
     <t>author of song lyrics</t>
   </si>
   <si>
@@ -558,39 +414,21 @@
     <t>subject's government</t>
   </si>
   <si>
-    <t>human culture or people (or several cultures) associated with this item</t>
-  </si>
-  <si>
-    <t>HDI value of a country</t>
-  </si>
-  <si>
     <t>person or item replaced</t>
   </si>
   <si>
-    <t>author of the libretto (words) of an opera, operetta, oratorio or cantata, or of the book of a musical</t>
-  </si>
-  <si>
-    <t>key of a musical composition</t>
-  </si>
-  <si>
     <t>standard nominal interval between scheduled or regularly recurring events</t>
   </si>
   <si>
     <t>measured dimension of an object</t>
   </si>
   <si>
-    <t>person or institution organizing an event</t>
-  </si>
-  <si>
     <t>located on the specified landform</t>
   </si>
   <si>
     <t>length of time of an event or process</t>
   </si>
   <si>
-    <t>patron saint adopted by the subject</t>
-  </si>
-  <si>
     <t>P132</t>
   </si>
   <si>
@@ -660,40 +498,550 @@
     <t>P165</t>
   </si>
   <si>
-    <t>P167</t>
-  </si>
-  <si>
-    <t>P168</t>
-  </si>
-  <si>
-    <t>P169</t>
-  </si>
-  <si>
-    <t>P173</t>
-  </si>
-  <si>
-    <t>P174</t>
-  </si>
-  <si>
-    <t>P177</t>
-  </si>
-  <si>
-    <t>P178</t>
-  </si>
-  <si>
-    <t>P180</t>
-  </si>
-  <si>
-    <t>P181</t>
-  </si>
-  <si>
-    <t>P182</t>
+    <t>member of</t>
+  </si>
+  <si>
+    <t>BTI Governance Index</t>
+  </si>
+  <si>
+    <t>BTI Status Index</t>
+  </si>
+  <si>
+    <t>ISNI</t>
+  </si>
+  <si>
+    <t>topic's main template</t>
+  </si>
+  <si>
+    <t>permanent duplicated item</t>
+  </si>
+  <si>
+    <t>participant in</t>
+  </si>
+  <si>
+    <t>maritime identification digits</t>
+  </si>
+  <si>
+    <t>age of majority</t>
+  </si>
+  <si>
+    <t>category for people who died here</t>
+  </si>
+  <si>
+    <t>motto</t>
+  </si>
+  <si>
+    <t>GS1 country code</t>
+  </si>
+  <si>
+    <t>WIPO ST.3</t>
+  </si>
+  <si>
+    <t>ISO 3166-1 numeric code</t>
+  </si>
+  <si>
+    <t>geoshape</t>
+  </si>
+  <si>
+    <t>marriageable age</t>
+  </si>
+  <si>
+    <t>compulsory education (maximum age)</t>
+  </si>
+  <si>
+    <t>demonym</t>
+  </si>
+  <si>
+    <t>subreddit</t>
+  </si>
+  <si>
+    <t>ISO 3166-1 alpha-2 code</t>
+  </si>
+  <si>
+    <t>Commons category</t>
+  </si>
+  <si>
+    <t>contains administrative territorial entity</t>
+  </si>
+  <si>
+    <t>suicide rate</t>
+  </si>
+  <si>
+    <t>GDP (PPP)</t>
+  </si>
+  <si>
+    <t>main regulatory text</t>
+  </si>
+  <si>
+    <t>railway traffic side</t>
+  </si>
+  <si>
+    <t>part of</t>
+  </si>
+  <si>
+    <t>on focus list of Wikimedia project</t>
+  </si>
+  <si>
+    <t>pronunciation audio</t>
+  </si>
+  <si>
+    <t>maintained by WikiProject</t>
+  </si>
+  <si>
+    <t>Swedish Anbytarforum</t>
+  </si>
+  <si>
+    <t>Wikimedia outline</t>
+  </si>
+  <si>
+    <t>CIVICUS Monitor country entry</t>
+  </si>
+  <si>
+    <t>IAB code</t>
+  </si>
+  <si>
+    <t>country calling code</t>
+  </si>
+  <si>
+    <t>total fertility rate</t>
+  </si>
+  <si>
+    <t>minimum temperature record</t>
+  </si>
+  <si>
+    <t>category for maps</t>
+  </si>
+  <si>
+    <t>literacy rate</t>
+  </si>
+  <si>
+    <t>flag</t>
+  </si>
+  <si>
+    <t>ethnic group</t>
+  </si>
+  <si>
+    <t>award received</t>
+  </si>
+  <si>
+    <t>driving side</t>
+  </si>
+  <si>
+    <t>Open Data portal</t>
+  </si>
+  <si>
+    <t>has quality</t>
+  </si>
+  <si>
+    <t>coordinate location</t>
+  </si>
+  <si>
+    <t>category for films shot at this location</t>
+  </si>
+  <si>
+    <t>IPA transcription</t>
+  </si>
+  <si>
+    <t>category of people buried here</t>
+  </si>
+  <si>
+    <t>category of associated people</t>
+  </si>
+  <si>
+    <t>lowest point</t>
+  </si>
+  <si>
+    <t>number of out-of-school children</t>
+  </si>
+  <si>
+    <t>real gross domestic product growth rate</t>
+  </si>
+  <si>
+    <t>life expectancy</t>
+  </si>
+  <si>
+    <t>Commons gallery</t>
+  </si>
+  <si>
+    <t>highest point</t>
+  </si>
+  <si>
+    <t>electrical plug type</t>
+  </si>
+  <si>
+    <t>page banner</t>
+  </si>
+  <si>
+    <t>nominal GDP</t>
+  </si>
+  <si>
+    <t>FIPS 10-4 (countries and regions)</t>
+  </si>
+  <si>
+    <t>significant event</t>
+  </si>
+  <si>
+    <t>geography of topic</t>
+  </si>
+  <si>
+    <t>VAT-rate</t>
+  </si>
+  <si>
+    <t>mains voltage</t>
+  </si>
+  <si>
+    <t>mobile country code</t>
+  </si>
+  <si>
+    <t>PPP GDP per capita</t>
+  </si>
+  <si>
+    <t>total reserves</t>
+  </si>
+  <si>
+    <t>official website</t>
+  </si>
+  <si>
+    <t>Dewey Decimal Classification</t>
+  </si>
+  <si>
+    <t>IOC country code</t>
+  </si>
+  <si>
+    <t>spoken text audio</t>
+  </si>
+  <si>
+    <t>topic's main category</t>
+  </si>
+  <si>
+    <t>history of topic</t>
+  </si>
+  <si>
+    <t>emergency phone number</t>
+  </si>
+  <si>
+    <t>unemployment rate</t>
+  </si>
+  <si>
+    <t>U.S. National Archives Identifier</t>
+  </si>
+  <si>
+    <t>OmegaWiki Defined Meaning</t>
+  </si>
+  <si>
+    <t>central bank</t>
+  </si>
+  <si>
+    <t>topic's main Wikimedia portal</t>
+  </si>
+  <si>
+    <t>coordinates of northernmost point</t>
+  </si>
+  <si>
+    <t>coordinates of southernmost point</t>
+  </si>
+  <si>
+    <t>coordinates of easternmost point</t>
+  </si>
+  <si>
+    <t>coordinates of westernmost point</t>
+  </si>
+  <si>
+    <t>water as percent of area</t>
+  </si>
+  <si>
+    <t>ISO 3166-2 code</t>
+  </si>
+  <si>
+    <t>Wolfram Language entity code</t>
+  </si>
+  <si>
+    <t>seal description</t>
+  </si>
+  <si>
+    <t>maximum temperature record</t>
+  </si>
+  <si>
+    <t>FIPS 5-2 alpha code (US states)</t>
+  </si>
+  <si>
+    <t>FIPS 5-2 numeric code (US states)</t>
+  </si>
+  <si>
+    <t>coordinates of geographic center</t>
+  </si>
+  <si>
+    <t>foundational text</t>
+  </si>
+  <si>
+    <t>named after</t>
+  </si>
+  <si>
+    <t>located in or next to body of water</t>
+  </si>
+  <si>
+    <t>located in the administrative territorial entity</t>
+  </si>
+  <si>
+    <t>HASC</t>
+  </si>
+  <si>
+    <t>nickname</t>
+  </si>
+  <si>
+    <t>Legal Entity Identifier</t>
+  </si>
+  <si>
+    <t>elevation above sea level</t>
+  </si>
+  <si>
+    <t>official symbol</t>
+  </si>
+  <si>
+    <t>said to be the same as</t>
+  </si>
+  <si>
+    <t>territory claimed by</t>
+  </si>
+  <si>
+    <t>place name sign</t>
+  </si>
+  <si>
+    <t>genre</t>
+  </si>
+  <si>
+    <t>cast member</t>
+  </si>
+  <si>
+    <t>creator</t>
+  </si>
+  <si>
+    <t>start time</t>
+  </si>
+  <si>
+    <t>original broadcaster</t>
+  </si>
+  <si>
+    <t>language of work or name</t>
+  </si>
+  <si>
+    <t>date of first performance</t>
+  </si>
+  <si>
+    <t>number of seasons</t>
+  </si>
+  <si>
+    <t>commemorates</t>
+  </si>
+  <si>
+    <t>day in year for periodic occurrence</t>
+  </si>
+  <si>
+    <t>foods traditionally associated</t>
+  </si>
+  <si>
+    <t>follows</t>
+  </si>
+  <si>
+    <t>followed by</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>hashtag</t>
+  </si>
+  <si>
+    <t>IPTC NewsCode</t>
+  </si>
+  <si>
+    <t>RIA Novosti reference</t>
+  </si>
+  <si>
+    <t>ICD-10</t>
+  </si>
+  <si>
+    <t>ICD-9</t>
+  </si>
+  <si>
+    <t>DiseasesDB</t>
+  </si>
+  <si>
+    <t>MeSH tree code</t>
+  </si>
+  <si>
+    <t>symptoms</t>
+  </si>
+  <si>
+    <t>Iconclass notation</t>
+  </si>
+  <si>
+    <t>exact match</t>
+  </si>
+  <si>
+    <t>UMLS CUI</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>genetic association</t>
+  </si>
+  <si>
+    <t>ICD-9-CM</t>
+  </si>
+  <si>
+    <t>ICD-10-CM</t>
+  </si>
+  <si>
+    <t>material used</t>
+  </si>
+  <si>
+    <t>Terminologia Histologica</t>
+  </si>
+  <si>
+    <t>TA98 Latin term</t>
+  </si>
+  <si>
+    <t>drug used for treatment</t>
+  </si>
+  <si>
+    <t>has part</t>
+  </si>
+  <si>
+    <t>Wikidata property</t>
+  </si>
+  <si>
+    <t>equivalent class</t>
+  </si>
+  <si>
+    <t>NUTS code</t>
+  </si>
+  <si>
+    <t>owner of</t>
+  </si>
+  <si>
+    <t>GSS code (2011)</t>
+  </si>
+  <si>
+    <t>Pleiades category identifier</t>
+  </si>
+  <si>
+    <t>UIC alphabetical country code</t>
+  </si>
+  <si>
+    <t>UIC numerical country code</t>
+  </si>
+  <si>
+    <t>ISBN identifier group</t>
+  </si>
+  <si>
+    <t>coextensive with</t>
+  </si>
+  <si>
+    <t>median income</t>
+  </si>
+  <si>
+    <t>studied by</t>
+  </si>
+  <si>
+    <t>individual tax rate</t>
+  </si>
+  <si>
+    <t>public holiday</t>
+  </si>
+  <si>
+    <t>Gregorian calendar start date</t>
+  </si>
+  <si>
+    <t>inflation rate</t>
+  </si>
+  <si>
+    <t>time of earliest written record</t>
+  </si>
+  <si>
+    <t>Hornbostel-Sachs classification</t>
+  </si>
+  <si>
+    <t>uses</t>
+  </si>
+  <si>
+    <t>described at URL</t>
+  </si>
+  <si>
+    <t>based on</t>
+  </si>
+  <si>
+    <t>WordLift URL</t>
+  </si>
+  <si>
+    <t>retirement age</t>
+  </si>
+  <si>
+    <t>M.49 code</t>
+  </si>
+  <si>
+    <t>audio</t>
+  </si>
+  <si>
+    <t>partially coincident with</t>
+  </si>
+  <si>
+    <t>location map</t>
+  </si>
+  <si>
+    <t>visitor centre</t>
+  </si>
+  <si>
+    <t>sex or gender</t>
+  </si>
+  <si>
+    <t>residence</t>
+  </si>
+  <si>
+    <t>spouse</t>
+  </si>
+  <si>
+    <t>inspired by</t>
+  </si>
+  <si>
+    <t>present in work</t>
+  </si>
+  <si>
+    <t>depicted by</t>
+  </si>
+  <si>
+    <t>child</t>
+  </si>
+  <si>
+    <t>occupation</t>
+  </si>
+  <si>
+    <t>performer</t>
+  </si>
+  <si>
+    <t>TV Tropes identifier</t>
+  </si>
+  <si>
+    <t>field of work</t>
+  </si>
+  <si>
+    <t>has cause</t>
+  </si>
+  <si>
+    <t>Basisklassifikation</t>
+  </si>
+  <si>
+    <t>opposite of</t>
+  </si>
+  <si>
+    <t>video</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1553,11 +1901,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E54" sqref="E2:E54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1568,29 +1916,33 @@
     <col min="4" max="4" width="7.5" customWidth="1"/>
     <col min="5" max="5" width="17.33203125" customWidth="1"/>
     <col min="6" max="6" width="104.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>125</v>
+        <v>87</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>126</v>
+        <v>88</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>127</v>
+        <v>89</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>128</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>129</v>
+        <v>91</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+      <c r="H1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1601,38 +1953,44 @@
         <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="E2" s="2" t="str">
         <f xml:space="preserve"> _xlfn.CONCAT("'", A2, "': '", D2, "',")</f>
         <v>'instance of': 'P130',</v>
       </c>
       <c r="F2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+      <c r="H2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="C3">
         <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E3" s="2" t="str">
-        <f t="shared" ref="E3:E54" si="0" xml:space="preserve"> _xlfn.CONCAT("'", A3, "': '", D3, "',")</f>
+        <f t="shared" ref="E3:E38" si="0" xml:space="preserve"> _xlfn.CONCAT("'", A3, "': '", D3, "',")</f>
         <v>'subclass of': 'P131',</v>
       </c>
       <c r="F3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="H3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1643,185 +2001,212 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>185</v>
+        <v>131</v>
       </c>
       <c r="E4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>'described by source': 'P132',</v>
       </c>
       <c r="F4" t="s">
+        <v>94</v>
+      </c>
+      <c r="H4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
         <v>132</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>186</v>
       </c>
       <c r="E5" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>'publication date': 'P133',</v>
+        <v>'inception': 'P133',</v>
       </c>
       <c r="F5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="H5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="C6">
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>187</v>
+        <v>133</v>
       </c>
       <c r="E6" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>'inception': 'P134',</v>
+        <v>'practiced by': 'P134',</v>
       </c>
       <c r="F6" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+      <c r="H6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>188</v>
+        <v>134</v>
       </c>
       <c r="E7" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>'composer': 'P135',</v>
+        <v>'anthem': 'P135',</v>
       </c>
       <c r="F7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+      <c r="H7" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>123</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>124</v>
+        <v>46</v>
       </c>
       <c r="C8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E8" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>'practiced by': 'P136',</v>
+        <v>'area': 'P136',</v>
       </c>
       <c r="F8" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+      <c r="H8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="E9" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>'copyright status': 'P137',</v>
+        <v>'capital': 'P137',</v>
       </c>
       <c r="F9" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+      <c r="H9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C10">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E10" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>'country': 'P138',</v>
+        <v>'continent': 'P138',</v>
       </c>
       <c r="F10" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="H10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C11">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>189</v>
+        <v>135</v>
       </c>
       <c r="E11" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>'head of government': 'P139',</v>
+        <v>'country': 'P139',</v>
       </c>
       <c r="F11" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+      <c r="H11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C12">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="E12" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>'legislative body': 'P140',</v>
+        <v>'currency': 'P140',</v>
       </c>
       <c r="F12" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+      <c r="H12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1832,190 +2217,217 @@
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>190</v>
+        <v>136</v>
       </c>
       <c r="E13" s="2" t="str">
         <f t="shared" si="0"/>
         <v>'executive body': 'P141',</v>
       </c>
       <c r="F13" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="H13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C14">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>191</v>
+        <v>137</v>
       </c>
       <c r="E14" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>'language used': 'P142',</v>
+        <v>'head of government': 'P142',</v>
       </c>
       <c r="F14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="H14" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>81</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="C15">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>192</v>
+        <v>138</v>
       </c>
       <c r="E15" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>'continent': 'P143',</v>
+        <v>'health specialty': 'P143',</v>
       </c>
       <c r="F15" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+      <c r="H15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C16">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="E16" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>'capital': 'P144',</v>
+        <v>'language used': 'P144',</v>
       </c>
       <c r="F16" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+      <c r="H16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C17">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>193</v>
+        <v>139</v>
       </c>
       <c r="E17" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>'official language': 'P145',</v>
+        <v>'legislative body': 'P145',</v>
       </c>
       <c r="F17" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+      <c r="H17" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C18">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>194</v>
+        <v>140</v>
       </c>
       <c r="E18" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>'currency': 'P146',</v>
+        <v>'located in time zone': 'P146',</v>
       </c>
       <c r="F18" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+      <c r="H18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="C19">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>195</v>
+        <v>141</v>
       </c>
       <c r="E19" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>'anthem': 'P147',</v>
+        <v>'native label': 'P147',</v>
       </c>
       <c r="F19" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+      <c r="H19" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="C20">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>196</v>
+        <v>142</v>
       </c>
       <c r="E20" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>'located in time zone': 'P148',</v>
+        <v>'nominal GDP per capita': 'P148',</v>
       </c>
       <c r="F20" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+      <c r="H20" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C21">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>197</v>
+        <v>143</v>
       </c>
       <c r="E21" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>'area': 'P149',</v>
+        <v>'office held by head of government': 'P149',</v>
       </c>
       <c r="F21" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+      <c r="H21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="C22">
         <v>4</v>
@@ -2025,691 +2437,1279 @@
       </c>
       <c r="E22" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>'short name': 'P150',</v>
+        <v>'official language': 'P150',</v>
       </c>
       <c r="F22" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+      <c r="H22" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C23">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>198</v>
+        <v>144</v>
       </c>
       <c r="E23" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>'nominal GDP per capita': 'P151',</v>
+        <v>'population': 'P151',</v>
       </c>
       <c r="F23" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+      <c r="H23" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C24">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>199</v>
+        <v>145</v>
       </c>
       <c r="E24" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>'population': 'P152',</v>
+        <v>'short name': 'P152',</v>
       </c>
       <c r="F24" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="H24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D25" t="s">
-        <v>200</v>
+        <v>146</v>
       </c>
       <c r="E25" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>'office held by head of government': 'P153',</v>
+        <v>'country of origin': 'P153',</v>
       </c>
       <c r="F25" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+      <c r="H25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="B26" t="s">
-        <v>67</v>
+        <v>19</v>
       </c>
       <c r="C26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D26" t="s">
-        <v>201</v>
+        <v>147</v>
       </c>
       <c r="E26" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>'native label': 'P154',</v>
+        <v>'head of state': 'P154',</v>
       </c>
       <c r="F26" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+      <c r="H26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B27" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C27">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D27" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="E27" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>'director': 'P155',</v>
+        <v>'highest judicial authority': 'P155',</v>
       </c>
       <c r="F27" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+      <c r="H27" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>103</v>
+        <v>43</v>
       </c>
       <c r="B28" t="s">
-        <v>104</v>
+        <v>44</v>
       </c>
       <c r="C28">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D28" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="E28" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>'location': 'P156',</v>
+        <v>'office held by head of state': 'P156',</v>
       </c>
       <c r="F28" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+      <c r="H28" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>119</v>
+        <v>22</v>
       </c>
       <c r="B29" t="s">
-        <v>120</v>
+        <v>23</v>
       </c>
       <c r="C29">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D29" t="s">
-        <v>202</v>
+        <v>148</v>
       </c>
       <c r="E29" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>'health specialty': 'P157',</v>
+        <v>'official name': 'P157',</v>
       </c>
       <c r="F29" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="H29" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B30" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C30">
         <v>3</v>
       </c>
       <c r="D30" t="s">
-        <v>203</v>
+        <v>149</v>
       </c>
       <c r="E30" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>'head of state': 'P158',</v>
+        <v>'shares border with': 'P158',</v>
       </c>
       <c r="F30" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="H30" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="C31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>204</v>
+        <v>150</v>
       </c>
       <c r="E31" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>'official name': 'P159',</v>
+        <v>'basic form of government': 'P159',</v>
       </c>
       <c r="F31" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+      <c r="H31" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="B32" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="C32">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D32" t="s">
-        <v>205</v>
+        <v>151</v>
       </c>
       <c r="E32" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>'shares border with': 'P160',</v>
+        <v>'culture': 'P160',</v>
       </c>
       <c r="F32" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+      <c r="H32" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>116</v>
+        <v>79</v>
       </c>
       <c r="E33" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>'office held by head of state': 'P161',</v>
+        <v>'diplomatic relation': 'P161',</v>
       </c>
       <c r="F33" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+      <c r="H33" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B34" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D34" t="s">
-        <v>117</v>
+        <v>80</v>
       </c>
       <c r="E34" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>'highest judicial authority': 'P162',</v>
+        <v>'Human Development Index': 'P162',</v>
       </c>
       <c r="F34" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+      <c r="H34" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="B35" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="C35">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D35" t="s">
         <v>39</v>
       </c>
       <c r="E35" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>'capital of': 'P163',</v>
+        <v>'located on terrain feature': 'P163',</v>
       </c>
       <c r="F35" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+      <c r="H35" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="B36" t="s">
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="C36">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D36" t="s">
-        <v>206</v>
+        <v>152</v>
       </c>
       <c r="E36" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>'screenwriter': 'P164',</v>
+        <v>'motto text': 'P164',</v>
       </c>
       <c r="F36" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+      <c r="H36" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B37" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="C37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D37" t="s">
-        <v>207</v>
+        <v>153</v>
       </c>
       <c r="E37" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>'original language of film or TV show': 'P165',</v>
+        <v>'patron saint': 'P165',</v>
       </c>
       <c r="F37" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+      <c r="H37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="B38" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C38">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E38" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>'country of origin': 'P166',</v>
+        <v>'replaces': 'P166',</v>
       </c>
       <c r="F38" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+        <v>130</v>
+      </c>
+      <c r="H38" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H39" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H40" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H41" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H42" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H43" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F44" s="3"/>
+      <c r="H44" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H45" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H46" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H47" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H48" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="49" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H49" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="50" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H50" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="51" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H51" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="52" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H52" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="53" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H53" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="54" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H54" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="55" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H55" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="56" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H56" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="57" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H57" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="58" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H58" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="59" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H59" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="60" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H60" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="61" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H61" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="62" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H62" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="63" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H63" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="64" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H64" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="65" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H65" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="66" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H66" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="67" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H67" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="68" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H68" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="69" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H69" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="70" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H70" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="71" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H71" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="72" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H72" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="73" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H73" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="74" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H74" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="75" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H75" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="76" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H76" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="77" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H77" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="78" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H78" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="79" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H79" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="80" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H80" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="81" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H81" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="82" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H82" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="83" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H83" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="84" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H84" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="85" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H85" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="86" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H86" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="87" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H87" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="88" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H88" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="89" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H89" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="90" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H90" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="91" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H91" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="92" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H92" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="93" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H93" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="94" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H94" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="95" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H95" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="96" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H96" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="97" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H97" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="98" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H98" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="99" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H99" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="100" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H100" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="101" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H101" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="102" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H102" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="103" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H103" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="104" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H104" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="105" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H105" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="106" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H106" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="107" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H107" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="108" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H108" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="109" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H109" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="110" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H110" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="111" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H111" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="112" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H112" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="113" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H113" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="114" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H114" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="115" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H115" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="116" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H116" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="117" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H117" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="118" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H118" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="119" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H119" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="120" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H120" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="121" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H121" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="122" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H122" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="123" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H123" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="124" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H124" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="125" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H125" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="126" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H126" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="127" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H127" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="128" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H128" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="129" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H129" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="130" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H130" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="131" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H131" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="132" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H132" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="133" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H133" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="134" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H134" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="135" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H135" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="136" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H136" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="137" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H137" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="138" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H138" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="139" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H139" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="140" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H140" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="141" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H141" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="142" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H142" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="143" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H143" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="144" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H144" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="145" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H145" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="146" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H146" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="147" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H147" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="148" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H148" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="149" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H149" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="150" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H150" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="151" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H151" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="152" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H152" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="153" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H153" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="154" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H154" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="155" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H155" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="156" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H156" t="s">
         <v>81</v>
       </c>
-      <c r="B39" t="s">
-        <v>82</v>
-      </c>
-      <c r="C39">
-        <v>3</v>
-      </c>
-      <c r="D39" t="s">
-        <v>208</v>
-      </c>
-      <c r="E39" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>'distributed by': 'P167',</v>
-      </c>
-      <c r="F39" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>96</v>
-      </c>
-      <c r="B40" t="s">
-        <v>97</v>
-      </c>
-      <c r="C40">
-        <v>3</v>
-      </c>
-      <c r="D40" t="s">
-        <v>209</v>
-      </c>
-      <c r="E40" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>'lyrics by': 'P168',</v>
-      </c>
-      <c r="F40" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>28</v>
-      </c>
-      <c r="B41" t="s">
-        <v>29</v>
-      </c>
-      <c r="C41">
-        <v>2</v>
-      </c>
-      <c r="D41" t="s">
-        <v>210</v>
-      </c>
-      <c r="E41" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>'motto text': 'P169',</v>
-      </c>
-      <c r="F41" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>32</v>
-      </c>
-      <c r="B42" t="s">
-        <v>33</v>
-      </c>
-      <c r="C42">
-        <v>2</v>
-      </c>
-      <c r="D42" t="s">
-        <v>118</v>
-      </c>
-      <c r="E42" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>'diplomatic relation': 'P170',</v>
-      </c>
-      <c r="F42" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>37</v>
-      </c>
-      <c r="B43" t="s">
-        <v>38</v>
-      </c>
-      <c r="C43">
-        <v>2</v>
-      </c>
-      <c r="D43" t="s">
-        <v>95</v>
-      </c>
-      <c r="E43" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>'basic form of government': 'P171',</v>
-      </c>
-      <c r="F43" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>48</v>
-      </c>
-      <c r="B44" t="s">
-        <v>49</v>
-      </c>
-      <c r="C44">
-        <v>2</v>
-      </c>
-      <c r="D44" t="s">
-        <v>40</v>
-      </c>
-      <c r="E44" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>'culture': 'P172',</v>
-      </c>
-      <c r="F44" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>54</v>
-      </c>
-      <c r="B45" t="s">
-        <v>55</v>
-      </c>
-      <c r="C45">
-        <v>2</v>
-      </c>
-      <c r="D45" t="s">
-        <v>211</v>
-      </c>
-      <c r="E45" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>'Human Development Index': 'P173',</v>
-      </c>
-      <c r="F45" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>64</v>
-      </c>
-      <c r="B46" t="s">
-        <v>65</v>
-      </c>
-      <c r="C46">
-        <v>2</v>
-      </c>
-      <c r="D46" t="s">
-        <v>212</v>
-      </c>
-      <c r="E46" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>'replaces': 'P174',</v>
-      </c>
-      <c r="F46" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>93</v>
-      </c>
-      <c r="B47" t="s">
-        <v>94</v>
-      </c>
-      <c r="C47">
-        <v>2</v>
-      </c>
-      <c r="D47" t="s">
-        <v>89</v>
-      </c>
-      <c r="E47" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>'librettist': 'P175',</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>99</v>
-      </c>
-      <c r="B48" t="s">
-        <v>100</v>
-      </c>
-      <c r="C48">
-        <v>2</v>
-      </c>
-      <c r="D48" t="s">
-        <v>106</v>
-      </c>
-      <c r="E48" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>'tonality': 'P176',</v>
-      </c>
-      <c r="F48" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>101</v>
-      </c>
-      <c r="B49" t="s">
-        <v>102</v>
-      </c>
-      <c r="C49">
-        <v>2</v>
-      </c>
-      <c r="D49" t="s">
-        <v>213</v>
-      </c>
-      <c r="E49" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>'event interval': 'P177',</v>
-      </c>
-      <c r="F49" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>107</v>
-      </c>
-      <c r="B50" t="s">
-        <v>108</v>
-      </c>
-      <c r="C50">
-        <v>2</v>
-      </c>
-      <c r="D50" t="s">
-        <v>214</v>
-      </c>
-      <c r="E50" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>'length': 'P178',</v>
-      </c>
-      <c r="F50" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>109</v>
-      </c>
-      <c r="B51" t="s">
-        <v>110</v>
-      </c>
-      <c r="C51">
-        <v>2</v>
-      </c>
-      <c r="D51" t="s">
-        <v>111</v>
-      </c>
-      <c r="E51" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>'organizer': 'P179',</v>
-      </c>
-      <c r="F51" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>112</v>
-      </c>
-      <c r="B52" t="s">
-        <v>113</v>
-      </c>
-      <c r="C52">
-        <v>2</v>
-      </c>
-      <c r="D52" t="s">
-        <v>215</v>
-      </c>
-      <c r="E52" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>'located on terrain feature': 'P180',</v>
-      </c>
-      <c r="F52" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>114</v>
-      </c>
-      <c r="B53" t="s">
-        <v>115</v>
-      </c>
-      <c r="C53">
-        <v>2</v>
-      </c>
-      <c r="D53" t="s">
-        <v>216</v>
-      </c>
-      <c r="E53" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>'duration': 'P181',</v>
-      </c>
-      <c r="F53" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>121</v>
-      </c>
-      <c r="B54" t="s">
-        <v>122</v>
-      </c>
-      <c r="C54">
-        <v>2</v>
-      </c>
-      <c r="D54" t="s">
-        <v>217</v>
-      </c>
-      <c r="E54" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>'patron saint': 'P182',</v>
-      </c>
-      <c r="F54" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F60" s="3"/>
+    </row>
+    <row r="157" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H157" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="158" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H158" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="159" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H159" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="160" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H160" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="161" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H161" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="162" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H162" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="163" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H163" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="164" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H164" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="165" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H165" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="166" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H166" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="167" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H167" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="168" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H168" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="169" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H169" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="170" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H170" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="171" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H171" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="172" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H172" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="173" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H173" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="174" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H174" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="175" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H175" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="176" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H176" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="177" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H177" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="178" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H178" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="179" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H179" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="180" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H180" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="181" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H181" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="182" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H182" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="183" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H183" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="184" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H184" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="185" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H185" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="186" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H186" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="187" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H187" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="188" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H188" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="189" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H189" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="190" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H190" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="191" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H191" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="192" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H192" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="193" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H193" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="194" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H194" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="195" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H195" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="196" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H196" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="197" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H197" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="198" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H198" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="199" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H199" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="200" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H200" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="201" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H201" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="202" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H202" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="203" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H203" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="204" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H204" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="205" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H205" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="206" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H206" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="207" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H207" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="208" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H208" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="209" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H209" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="210" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H210" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="211" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H211" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="212" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H212" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="213" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H213" t="s">
+        <v>333</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C1">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C378">
-      <sortCondition descending="1" ref="C1:C378"/>
+  <autoFilter ref="A1:C1" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C54">
+      <sortCondition descending="1" ref="C1:C54"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="20" type="noConversion"/>

</xml_diff>